<commit_message>
[UEAT] System event log dump and database data upload
Update the function of autoly dump system event and filter specific event ids, and also the function of upload the test result to the remote database.
</commit_message>
<xml_diff>
--- a/user_exp_auto_test_ui/database_data.xlsx
+++ b/user_exp_auto_test_ui/database_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benlaix\auto_workspace\auto_test\user_exp_auto_test_ui\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\auto_workspace\auto_test\user_exp_auto_test_ui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CF4E58-189F-4D18-8BAE-004FF4C65C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F7E5C1-9A3F-4649-A0C3-0009CDBADDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42479C74-CFC1-49C4-852C-6237A10D3325}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{42479C74-CFC1-49C4-852C-6237A10D3325}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -1328,19 +1328,19 @@
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.81640625" customWidth="1"/>
-    <col min="3" max="3" width="35.7265625" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.1796875" customWidth="1"/>
-    <col min="6" max="6" width="37.6328125" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="36" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>97</v>
@@ -1361,7 +1361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A66" si="0">A2+1</f>
         <v>2</v>
@@ -1402,7 +1402,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="25"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1424,7 +1424,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1442,7 +1442,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="25"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1462,7 +1462,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="25"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1479,12 +1479,10 @@
       <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>186</v>
-      </c>
+      <c r="F7" s="7"/>
       <c r="G7" s="25"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1503,7 +1501,7 @@
       </c>
       <c r="G8" s="25"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1525,7 +1523,7 @@
       </c>
       <c r="G9" s="25"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1545,7 +1543,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="25"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1565,7 +1563,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="25"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1585,7 +1583,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="25"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1605,7 +1603,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="25"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1622,12 +1620,9 @@
       <c r="E14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="22" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" s="25"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1644,10 +1639,12 @@
       <c r="E15" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1667,7 +1664,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="25"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1687,7 +1684,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1707,7 +1704,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="25"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1727,7 +1724,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="25"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1747,7 +1744,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="25"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1762,7 +1759,7 @@
       <c r="E21" s="2"/>
       <c r="G21" s="25"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1782,7 +1779,7 @@
       </c>
       <c r="G22" s="25"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1800,7 +1797,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="25"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1817,7 +1814,7 @@
       <c r="E24" s="2"/>
       <c r="G24" s="25"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1839,7 +1836,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1856,7 +1853,7 @@
       <c r="E26" s="2"/>
       <c r="G26" s="33"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1876,7 +1873,7 @@
       </c>
       <c r="G27" s="25"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1894,7 +1891,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="25"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1916,7 +1913,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1931,7 +1928,7 @@
       <c r="E30" s="2"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1951,7 +1948,7 @@
       </c>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1969,7 +1966,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1988,7 +1985,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2010,7 +2007,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2030,7 +2027,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2052,7 +2049,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2072,7 +2069,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2090,7 +2087,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2110,7 +2107,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2130,7 +2127,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2150,7 +2147,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2170,7 +2167,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2192,7 +2189,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2212,7 +2209,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2232,7 +2229,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2250,7 +2247,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2270,7 +2267,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2290,7 +2287,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2308,7 +2305,7 @@
       <c r="F49" s="20"/>
       <c r="G49" s="25"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2328,7 +2325,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2348,7 +2345,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -2368,7 +2365,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -2388,7 +2385,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -2408,7 +2405,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -2426,7 +2423,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -2444,7 +2441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -2464,7 +2461,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -2484,7 +2481,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -2504,7 +2501,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -2524,7 +2521,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -2544,7 +2541,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -2564,7 +2561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -2586,7 +2583,7 @@
       </c>
       <c r="G63" s="25"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -2608,7 +2605,7 @@
       </c>
       <c r="G64" s="32"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -2626,7 +2623,7 @@
       <c r="F65" s="33"/>
       <c r="G65" s="33"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -2644,7 +2641,7 @@
       <c r="F66" s="33"/>
       <c r="G66" s="33"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <f t="shared" ref="A67:A69" si="1">A66+1</f>
         <v>66</v>
@@ -2660,7 +2657,7 @@
       <c r="F67" s="33"/>
       <c r="G67" s="33"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -2676,7 +2673,7 @@
       <c r="F68" s="33"/>
       <c r="G68" s="33"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <f t="shared" si="1"/>
         <v>68</v>

</xml_diff>

<commit_message>
[UEAT] WRT warning code detected
1. Add WRT warning code detected function
2. modify the name of wifi band
</commit_message>
<xml_diff>
--- a/user_exp_auto_test_ui/database_data.xlsx
+++ b/user_exp_auto_test_ui/database_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="196">
   <si>
     <t>Name</t>
   </si>
@@ -588,7 +588,22 @@
     <t>OFF</t>
   </si>
   <si>
+    <t>Wi-Fi Band</t>
+  </si>
+  <si>
     <t>wifi_band</t>
+  </si>
+  <si>
+    <t>System event log</t>
+  </si>
+  <si>
+    <t>sys_event_log</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -818,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -941,6 +956,9 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2536,10 +2554,10 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D71" s="40" t="s">
         <v>189</v>
@@ -2548,8 +2566,40 @@
       <c r="F71" s="41"/>
       <c r="G71" s="41"/>
     </row>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1">
+      <c r="A72" s="39">
+        <v>71.0</v>
+      </c>
+      <c r="B72" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
+      <c r="F72" s="41"/>
+      <c r="G72" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" ht="14.25" customHeight="1">
+      <c r="A73" s="39">
+        <v>72.0</v>
+      </c>
+      <c r="B73" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
+      <c r="F73" s="41"/>
+      <c r="G73" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="74" ht="14.25" customHeight="1"/>
     <row r="75" ht="14.25" customHeight="1"/>
     <row r="76" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
[UEAT] Modify WRT code filter
1. Modify the wrt code filter
2. Modify the safe clicking function
3. Modify the database info wifi band getting function
</commit_message>
<xml_diff>
--- a/user_exp_auto_test_ui/database_data.xlsx
+++ b/user_exp_auto_test_ui/database_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>LE</t>
+  </si>
+  <si>
+    <t>LE,Classic</t>
   </si>
   <si>
     <t>Mouse</t>
@@ -882,6 +885,9 @@
     <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -948,9 +954,6 @@
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -1636,8 +1639,12 @@
       <c r="D23" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="8"/>
+      <c r="E23" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -1646,13 +1653,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3"/>
       <c r="G24" s="6"/>
@@ -1663,17 +1670,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D25" s="3">
         <v>3.0</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="16" t="s">
-        <v>77</v>
+      <c r="F25" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>9</v>
@@ -1685,16 +1692,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>71</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="G26" s="17"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
       <c r="A27" s="3">
@@ -1702,10 +1709,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>67</v>
@@ -1722,13 +1729,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="8"/>
@@ -1740,17 +1747,17 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" s="3">
         <v>3.0</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>9</v>
@@ -1762,10 +1769,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1777,13 +1784,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="14" t="s">
@@ -1797,15 +1804,15 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="E32" s="19"/>
       <c r="F32" s="8"/>
       <c r="G32" s="6"/>
     </row>
@@ -1815,15 +1822,15 @@
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" s="18"/>
+        <v>98</v>
+      </c>
+      <c r="E33" s="19"/>
       <c r="G33" s="6" t="s">
         <v>9</v>
       </c>
@@ -1834,15 +1841,15 @@
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="18"/>
+        <v>101</v>
+      </c>
+      <c r="E34" s="19"/>
       <c r="F34" s="14" t="s">
         <v>68</v>
       </c>
@@ -1856,15 +1863,15 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="18"/>
+        <v>104</v>
+      </c>
+      <c r="E35" s="19"/>
       <c r="F35" s="8"/>
       <c r="G35" s="3" t="s">
         <v>9</v>
@@ -1876,15 +1883,15 @@
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="19"/>
+        <v>107</v>
+      </c>
+      <c r="E36" s="20"/>
       <c r="F36" s="14" t="s">
         <v>68</v>
       </c>
@@ -1898,16 +1905,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20"/>
+        <v>110</v>
+      </c>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="6" t="s">
         <v>9</v>
       </c>
@@ -1918,14 +1925,14 @@
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="23"/>
       <c r="G38" s="3" t="s">
         <v>9</v>
       </c>
@@ -1936,16 +1943,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+        <v>115</v>
+      </c>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="6" t="s">
         <v>9</v>
       </c>
@@ -1956,15 +1963,15 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="23"/>
+        <v>118</v>
+      </c>
+      <c r="E40" s="24"/>
       <c r="F40" s="5"/>
       <c r="G40" s="6" t="s">
         <v>9</v>
@@ -1976,10 +1983,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D41" s="3">
         <v>3.0</v>
@@ -1996,10 +2003,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C42" s="24" t="s">
         <v>121</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>122</v>
       </c>
       <c r="D42" s="3">
         <v>4.0</v>
@@ -2016,17 +2023,17 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>9</v>
@@ -2038,10 +2045,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D44" s="3">
         <v>3.0</v>
@@ -2058,10 +2065,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="24" t="s">
         <v>129</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>130</v>
       </c>
       <c r="D45" s="3">
         <v>4.0</v>
@@ -2078,10 +2085,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C46" s="24" t="s">
         <v>131</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>132</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
@@ -2096,10 +2103,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D47" s="3">
         <v>3.0</v>
@@ -2116,10 +2123,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="24" t="s">
         <v>135</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="D48" s="3">
         <v>4.0</v>
@@ -2136,13 +2143,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
@@ -2154,16 +2161,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" s="25"/>
-      <c r="F50" s="26"/>
+        <v>125</v>
+      </c>
+      <c r="E50" s="26"/>
+      <c r="F50" s="27"/>
       <c r="G50" s="6" t="s">
         <v>9</v>
       </c>
@@ -2174,10 +2181,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D51" s="3">
         <v>3.0</v>
@@ -2194,16 +2201,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="24" t="s">
         <v>143</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>144</v>
       </c>
       <c r="D52" s="3">
         <v>4.0</v>
       </c>
-      <c r="E52" s="18"/>
-      <c r="F52" s="27"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="28"/>
       <c r="G52" s="6" t="s">
         <v>9</v>
       </c>
@@ -2214,16 +2221,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="29"/>
+        <v>118</v>
+      </c>
+      <c r="E53" s="29"/>
+      <c r="F53" s="30"/>
       <c r="G53" s="6" t="s">
         <v>9</v>
       </c>
@@ -2234,10 +2241,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D54" s="8">
         <v>3.0</v>
@@ -2254,14 +2261,14 @@
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" s="30"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+        <v>150</v>
+      </c>
+      <c r="D55" s="31"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
       <c r="G55" s="6" t="s">
         <v>9</v>
       </c>
@@ -2272,14 +2279,14 @@
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
+        <v>152</v>
+      </c>
+      <c r="D56" s="31"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
       <c r="G56" s="6" t="s">
         <v>9</v>
       </c>
@@ -2290,16 +2297,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
+        <v>155</v>
+      </c>
+      <c r="E57" s="32"/>
+      <c r="F57" s="33"/>
       <c r="G57" s="6" t="s">
         <v>9</v>
       </c>
@@ -2310,16 +2317,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D58" s="3">
         <v>300.0</v>
       </c>
-      <c r="E58" s="33"/>
-      <c r="F58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
       <c r="G58" s="6" t="s">
         <v>9</v>
       </c>
@@ -2329,17 +2336,17 @@
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="B59" s="35" t="s">
-        <v>157</v>
-      </c>
-      <c r="C59" s="35" t="s">
+      <c r="B59" s="36" t="s">
         <v>158</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>159</v>
       </c>
       <c r="D59" s="3">
         <v>16.0</v>
       </c>
-      <c r="E59" s="33"/>
-      <c r="F59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="35"/>
       <c r="G59" s="6" t="s">
         <v>9</v>
       </c>
@@ -2350,16 +2357,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D60" s="3">
         <v>2.0</v>
       </c>
-      <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
       <c r="G60" s="6" t="s">
         <v>9</v>
       </c>
@@ -2369,17 +2376,17 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B61" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C61" s="37" t="s">
+      <c r="B61" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="C61" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="E61" s="33"/>
-      <c r="F61" s="34"/>
+      <c r="D61" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
       <c r="G61" s="6" t="s">
         <v>9</v>
       </c>
@@ -2390,16 +2397,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E62" s="33"/>
-      <c r="F62" s="34"/>
+        <v>167</v>
+      </c>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
       <c r="G62" s="6" t="s">
         <v>9</v>
       </c>
@@ -2409,20 +2416,20 @@
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="B63" s="35" t="s">
-        <v>167</v>
+      <c r="B63" s="36" t="s">
+        <v>168</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="33" t="s">
-        <v>170</v>
+      <c r="F63" s="34" t="s">
+        <v>171</v>
       </c>
       <c r="G63" s="6"/>
     </row>
@@ -2431,119 +2438,119 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-      <c r="B64" s="35" t="s">
-        <v>171</v>
+      <c r="B64" s="36" t="s">
+        <v>172</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F64" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G64" s="38"/>
+        <v>175</v>
+      </c>
+      <c r="G64" s="39"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="3">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="B65" s="35" t="s">
-        <v>175</v>
+      <c r="B65" s="36" t="s">
+        <v>176</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
+        <v>178</v>
+      </c>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
     </row>
     <row r="66" ht="14.25" customHeight="1">
       <c r="A66" s="3">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="B66" s="35" t="s">
-        <v>178</v>
+      <c r="B66" s="36" t="s">
+        <v>179</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
+        <v>181</v>
+      </c>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+      <c r="G66" s="18"/>
     </row>
     <row r="67" ht="14.25" customHeight="1">
       <c r="A67" s="3">
         <f t="shared" si="1"/>
         <v>66</v>
       </c>
-      <c r="B67" s="35" t="s">
-        <v>181</v>
+      <c r="B67" s="36" t="s">
+        <v>182</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D67" s="8"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="17"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
+      <c r="G67" s="18"/>
     </row>
     <row r="68" ht="14.25" customHeight="1">
       <c r="A68" s="3">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="B68" s="35" t="s">
-        <v>183</v>
+      <c r="B68" s="36" t="s">
+        <v>184</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D68" s="8"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="17"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
     </row>
     <row r="69" ht="14.25" customHeight="1">
       <c r="A69" s="3">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B69" s="35" t="s">
-        <v>185</v>
+      <c r="B69" s="36" t="s">
+        <v>186</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D69" s="8"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="17"/>
-      <c r="G69" s="17"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
     </row>
     <row r="70" ht="14.25" customHeight="1">
       <c r="A70" s="3">
         <v>69.0</v>
       </c>
-      <c r="B70" s="39" t="s">
-        <v>187</v>
+      <c r="B70" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D70" s="40" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E70" s="41"/>
       <c r="F70" s="41"/>
@@ -2553,28 +2560,28 @@
       <c r="A71" s="3">
         <v>70.0</v>
       </c>
-      <c r="B71" s="39" t="s">
+      <c r="B71" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" s="40" t="s">
         <v>190</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D71" s="40" t="s">
-        <v>189</v>
       </c>
       <c r="E71" s="41"/>
       <c r="F71" s="41"/>
       <c r="G71" s="41"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
-      <c r="A72" s="39">
+      <c r="A72" s="16">
         <v>71.0</v>
       </c>
       <c r="B72" s="42" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D72" s="41"/>
       <c r="E72" s="41"/>
@@ -2584,14 +2591,14 @@
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
-      <c r="A73" s="39">
+      <c r="A73" s="16">
         <v>72.0</v>
       </c>
       <c r="B73" s="42" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D73" s="41"/>
       <c r="E73" s="41"/>

</xml_diff>

<commit_message>
[UEAT] Add the wrt preset and ver getting function
1. database default value setting
2. wrt ver and preset getting
3. filter build-in mouse and keyboard
</commit_message>
<xml_diff>
--- a/user_exp_auto_test_ui/database_data.xlsx
+++ b/user_exp_auto_test_ui/database_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -105,7 +105,7 @@
     <t>PV</t>
   </si>
   <si>
-    <t>EVT, DVT1, DVT2,PV, MP</t>
+    <t>EVT, DVT1, DVT2,PV, MP,other</t>
   </si>
   <si>
     <t>Platform BIOS</t>
@@ -162,7 +162,7 @@
     <t>PCIe</t>
   </si>
   <si>
-    <t>USB,PCIe</t>
+    <t>USB,PCIe,other</t>
   </si>
   <si>
     <t>WiFi Deiver</t>
@@ -222,7 +222,7 @@
     <t>Logitech</t>
   </si>
   <si>
-    <t>Microsoft,Logitech, Samsung, Asus,Dell,Sony,HP,None</t>
+    <t>Microsoft,Logitech, Samsung, Asus,Dell,Sony,HP,other,None</t>
   </si>
   <si>
     <t>Mouse BT</t>
@@ -234,7 +234,7 @@
     <t>LE</t>
   </si>
   <si>
-    <t>LE,Classic</t>
+    <t>LE,Classic,None</t>
   </si>
   <si>
     <t>Mouse</t>
@@ -531,7 +531,7 @@
     <t>AC/DC</t>
   </si>
   <si>
-    <t>AC, DC</t>
+    <t xml:space="preserve"> DC,AC</t>
   </si>
   <si>
     <t>Urgent Level</t>
@@ -543,7 +543,7 @@
     <t>P2</t>
   </si>
   <si>
-    <t>Fireball , P1 , P2 , P3,None</t>
+    <t>None,Fireball , P1 , P2 , P3,other</t>
   </si>
   <si>
     <t>Plan to fix in WW</t>
@@ -836,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -867,6 +867,9 @@
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -878,9 +881,6 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -951,6 +951,9 @@
     </xf>
     <xf borderId="1" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1364,7 +1367,7 @@
       <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="G9" s="6"/>
@@ -1473,19 +1476,19 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="12" t="s">
         <v>48</v>
       </c>
       <c r="G15" s="6"/>
@@ -1598,10 +1601,10 @@
       <c r="B21" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="3"/>
       <c r="G21" s="6"/>
     </row>
@@ -1610,17 +1613,17 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="10" t="s">
         <v>68</v>
       </c>
       <c r="G22" s="6"/>
@@ -1636,13 +1639,13 @@
       <c r="C23" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="14" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="10" t="s">
         <v>72</v>
       </c>
       <c r="G23" s="6"/>
@@ -1697,10 +1700,15 @@
       <c r="C26" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="G26" s="18"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
@@ -1708,17 +1716,17 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>67</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="10" t="s">
         <v>68</v>
       </c>
       <c r="G27" s="6"/>
@@ -1755,7 +1763,7 @@
       <c r="D29" s="3">
         <v>3.0</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="8" t="s">
         <v>78</v>
       </c>
@@ -1775,7 +1783,12 @@
         <v>89</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="E30" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="G30" s="6"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
@@ -1783,17 +1796,17 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="14" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="10" t="s">
         <v>68</v>
       </c>
       <c r="G31" s="6"/>
@@ -1827,7 +1840,7 @@
       <c r="C33" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="14" t="s">
         <v>98</v>
       </c>
       <c r="E33" s="19"/>
@@ -1840,17 +1853,17 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>101</v>
       </c>
       <c r="E34" s="19"/>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="10" t="s">
         <v>68</v>
       </c>
       <c r="G34" s="6" t="s">
@@ -1882,17 +1895,17 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="14" t="s">
         <v>107</v>
       </c>
       <c r="E36" s="20"/>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="10" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="6" t="s">
@@ -1924,10 +1937,10 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>112</v>
       </c>
       <c r="D38" s="3"/>
@@ -2428,7 +2441,7 @@
       <c r="E63" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="34" t="s">
+      <c r="F63" s="39" t="s">
         <v>171</v>
       </c>
       <c r="G63" s="6"/>
@@ -2450,10 +2463,10 @@
       <c r="E64" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="G64" s="39"/>
+      <c r="G64" s="40"/>
     </row>
     <row r="65" ht="14.25" customHeight="1">
       <c r="A65" s="3">
@@ -2549,12 +2562,12 @@
       <c r="C70" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="40" t="s">
+      <c r="D70" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="E70" s="41"/>
-      <c r="F70" s="41"/>
-      <c r="G70" s="41"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="42"/>
     </row>
     <row r="71" ht="14.25" customHeight="1">
       <c r="A71" s="3">
@@ -2566,26 +2579,26 @@
       <c r="C71" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D71" s="40" t="s">
+      <c r="D71" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="E71" s="41"/>
-      <c r="F71" s="41"/>
-      <c r="G71" s="41"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="42"/>
     </row>
     <row r="72" ht="14.25" customHeight="1">
       <c r="A72" s="16">
         <v>71.0</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="43" t="s">
         <v>193</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
-      <c r="F72" s="41"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
+      <c r="F72" s="42"/>
       <c r="G72" s="6" t="s">
         <v>9</v>
       </c>
@@ -2594,15 +2607,15 @@
       <c r="A73" s="16">
         <v>72.0</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="41"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
+      <c r="F73" s="42"/>
       <c r="G73" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
[UEAT] Add new patten and new database item
1. Add S3+mouse+audio patten
2. Add music_type database item
3. Database item: teams <-- auto filled
</commit_message>
<xml_diff>
--- a/user_exp_auto_test_ui/database_data.xlsx
+++ b/user_exp_auto_test_ui/database_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Music type</t>
+  </si>
+  <si>
+    <t>music_type</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -673,6 +682,11 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -836,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -964,6 +978,9 @@
     <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2620,7 +2637,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1">
+      <c r="A74" s="16">
+        <v>73.0</v>
+      </c>
+      <c r="B74" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
+      <c r="G74" s="44" t="s">
+        <v>199</v>
+      </c>
+    </row>
     <row r="75" ht="14.25" customHeight="1"/>
     <row r="76" ht="14.25" customHeight="1"/>
     <row r="77" ht="14.25" customHeight="1"/>

</xml_diff>